<commit_message>
Added final documentation for project
</commit_message>
<xml_diff>
--- a/Planetarium Documentation/Planetarium Requirements Documentation.xlsx
+++ b/Planetarium Documentation/Planetarium Requirements Documentation.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="150">
   <si>
     <t>Users should be able to open a new User account with the Planetarium</t>
   </si>
@@ -57,6 +57,9 @@
     <t>Usernames should not be longer than 30 characters</t>
   </si>
   <si>
+    <t>Given a user is on the Login screen in Planetarium</t>
+  </si>
+  <si>
     <t>Moons should be “owned” by the Planet the User adding the moon associated it with</t>
   </si>
   <si>
@@ -69,16 +72,25 @@
     <t>Passwords should not be longer than 30 characters</t>
   </si>
   <si>
+    <t>When a user inputs a valid username before selecting the Login button</t>
+  </si>
+  <si>
     <t>Planets and Moons should allow adding an associated image, but an image should not be required for the data to be added to the database</t>
   </si>
   <si>
+    <t>Given a user has selected Planet on the Planetarium home page</t>
+  </si>
+  <si>
     <t>Planets and moons should have unique names</t>
   </si>
   <si>
+    <t>Given the user selected Moon on the Planetarium home page</t>
+  </si>
+  <si>
     <t>Given a user is on the Create Account screen in Planetarium</t>
   </si>
   <si>
-    <t>Given a user is on the Login screen in Planetarium</t>
+    <t>When a user inputs a valid password before selecting the Login button</t>
   </si>
   <si>
     <t>Given a user is on the home page in Planetarium</t>
@@ -87,16 +99,16 @@
     <t>Planets should allow adding an associated image, but an image should not be required for the data to be added to the database</t>
   </si>
   <si>
-    <t>Given a user has selected Planet on the Planetarium home page</t>
-  </si>
-  <si>
-    <t>Given the user selected Moon on the Planetarium home page</t>
+    <t>When the user inputs a name of a Planet that they own before selecting the Delete button</t>
+  </si>
+  <si>
+    <t>When the user inputs a name of a Moon that they own before selecting the Delete button</t>
   </si>
   <si>
     <t>When a user inputs an unique username before selecting the Create button</t>
   </si>
   <si>
-    <t>When a user inputs a valid username before selecting the Login button</t>
+    <t>Then the user is redirected to their home page</t>
   </si>
   <si>
     <t>Then the user should see all the planets and moons they added to Planetarium</t>
@@ -105,34 +117,25 @@
     <t>Given a user has selected Planet on the Plantarium home page</t>
   </si>
   <si>
-    <t>When the user inputs a name of a Planet that they own before selecting the Delete button</t>
-  </si>
-  <si>
-    <t>When the user inputs a name of a Moon that they own before selecting the Delete button</t>
+    <t>Then the home page should refresh to no longer display the Planet and Moons tied to the Planet that were deleted</t>
+  </si>
+  <si>
+    <t>Then the home page should refresh to no longer display the Moon that was deleted</t>
   </si>
   <si>
     <t>When a user inputs a username shorter than or equal to 30 characters before selecting the Create button</t>
   </si>
   <si>
-    <t>When a user inputs a valid password before selecting the Login button</t>
-  </si>
-  <si>
     <t>When the user inputs an unique name for the Planet before selecting the Submit Planet button</t>
   </si>
   <si>
-    <t>Then the home page should refresh to no longer display the Planet and Moons tied to the Planet that were deleted</t>
-  </si>
-  <si>
     <t>Given a user has selected Moon on the Planetarium home page</t>
   </si>
   <si>
-    <t>Then the home page should refresh to no longer display the Moon that was deleted</t>
-  </si>
-  <si>
     <t>When a user inputs a password shorter than or equal to 30 characters before selecting the Create button</t>
   </si>
   <si>
-    <t>Then the user is redirected to their home page</t>
+    <t>When a user inputs an invalid username before selecting the Login button</t>
   </si>
   <si>
     <t>When the user notices a planet/moon not owned by the user</t>
@@ -141,9 +144,15 @@
     <t>When the user inputs a name for the Planet that is less than or equal to 30 characters long before selecting the Submit Planet button</t>
   </si>
   <si>
+    <t>When the user inputs a name of a Planet that doesn't exist before selecting the Delete button</t>
+  </si>
+  <si>
     <t>When the user inputs an unique name for the Moon before selecting the Submit Moon button</t>
   </si>
   <si>
+    <t>When the user inputs a name of a Moon that doesn't exist before selecting the Delete button</t>
+  </si>
+  <si>
     <t>Then a notification is given to the user that their account with username is created successfully and the user is redirected back to the Login screen</t>
   </si>
   <si>
@@ -153,16 +162,16 @@
     <t>When the user inputs an image file for the Planet before selecting the Submit Planet button</t>
   </si>
   <si>
-    <t>When the user inputs a name of a Planet that doesn't exist before selecting the Delete button</t>
+    <t>When the user inputs a name of a Planet that is not owned by the user before selecting the Delete button</t>
   </si>
   <si>
     <t>When the user inputs a name for the Moon that is less than or equal to 30 characters before selecting the Submit Moon button</t>
   </si>
   <si>
-    <t>When the user inputs a name of a Moon that doesn't exist before selecting the Delete button</t>
-  </si>
-  <si>
-    <t>When a user inputs an invalid username before selecting the Login button</t>
+    <t>When the user inputs a name of a Moon that the user does not own before selecting the Delete button</t>
+  </si>
+  <si>
+    <t>Then the user is given a notification their login attempt failed</t>
   </si>
   <si>
     <t>Given a user has created a Planet</t>
@@ -171,37 +180,34 @@
     <t>Or the user doesn't input an image file for the Planet before selecting the Submit Planet button</t>
   </si>
   <si>
-    <t>When the user inputs a name of a Planet that is not owned by the user before selecting the Delete button</t>
+    <t>Then a notification should be given to the user that Planet deletion has failed</t>
   </si>
   <si>
     <t>When the user inputs an image file for the Moon before selecting the Submit Moon button</t>
   </si>
   <si>
-    <t>When the user inputs a name of a Moon that the user does not own before selecting the Delete button</t>
+    <t>Then a notification should be given to the user that Moon deletion has failed</t>
   </si>
   <si>
     <t>When a user inputs a username that has been used before (not unique) before selecting the Create button</t>
   </si>
   <si>
+    <t>Given a user is accessing the home page via "/planetarium"</t>
+  </si>
+  <si>
     <t>When the data for the Planet is valid</t>
   </si>
   <si>
     <t>Then the home page should refresh to display the newly created Planet for the user</t>
   </si>
   <si>
-    <t>Then a notification should be given to the user that Planet deletion has failed</t>
-  </si>
-  <si>
     <t>Or the user doesn't input an image file for the Moon before selecting the Submit Moon button</t>
   </si>
   <si>
-    <t>Then a notification should be given to the user that Moon deletion has failed</t>
-  </si>
-  <si>
     <t>When a user inputs a blank username before selecting the Create button</t>
   </si>
   <si>
-    <t>Then the user is given a notification their login attempt failed</t>
+    <t>When the user has logged in previously via session data</t>
   </si>
   <si>
     <t>Then the user should be able to see the newly created Planet on the home page</t>
@@ -216,7 +222,7 @@
     <t>When a user inputs a username that is greater than 30 characters before selecting the Create button</t>
   </si>
   <si>
-    <t>Given a user is accessing the home page via "/planetarium"</t>
+    <t>Then the user should be redirected to their home page</t>
   </si>
   <si>
     <t>Given a user has created a Moon</t>
@@ -231,9 +237,6 @@
     <t>When a user inputs a blank password before selecting the Create button</t>
   </si>
   <si>
-    <t>When the user has logged in previously via session data</t>
-  </si>
-  <si>
     <t>When the data and Planet for the Moon is valid</t>
   </si>
   <si>
@@ -243,7 +246,7 @@
     <t>When a user inputs a password that is greater than 30 characters before selecting the Create button</t>
   </si>
   <si>
-    <t>Then the user should be redirected to their home page</t>
+    <t>When the user has not logged in previously (i.e recently signed out) via session data</t>
   </si>
   <si>
     <t>Then the user should be able to see the newly created Moon on the home page</t>
@@ -258,6 +261,9 @@
     <t>Then a notification is given to the user that their account with username failed to be created</t>
   </si>
   <si>
+    <t>Then the user should be informed to log in prior to accessing the home page</t>
+  </si>
+  <si>
     <t>Given a user has deleted a Planet</t>
   </si>
   <si>
@@ -267,15 +273,9 @@
     <t>When the user inputs a blank name for the Moon before selecting the Submit Moon button</t>
   </si>
   <si>
-    <t>When the user has not logged in previously (i.e recently signed out) via session data</t>
-  </si>
-  <si>
     <t>When the user inputs a name for the Moon that is greater than 30 characters before selecting the Submit Moon button</t>
   </si>
   <si>
-    <t>Then the user should be informed to log in prior to accessing the home page</t>
-  </si>
-  <si>
     <t>Then the user should see that the deleted Planet and its Moons is no longer on the home page</t>
   </si>
   <si>
@@ -297,9 +297,27 @@
     <t>Then the user should see that the deleted Moon is no longer on the home page</t>
   </si>
   <si>
+    <t>Exploratary testing would be used to check if passwords are not stored in the database after account creation</t>
+  </si>
+  <si>
+    <t>Exploratary testing would be used to check if passwords are not in plaintext when being transported across the application</t>
+  </si>
+  <si>
     <t>Error Guess testing would be used to check if an user can see their planets and moons when a user accesses their home page</t>
   </si>
   <si>
+    <t>Exploratary testing would be used to see if a user's planet is added to the database upon successful creation</t>
+  </si>
+  <si>
+    <t>Exploratary testing would be used to see if a user's planet and its moons are removed from the database upon successful deletion</t>
+  </si>
+  <si>
+    <t>Exploratary testing would be used to see if a user's moon is added to the database upon successful creation</t>
+  </si>
+  <si>
+    <t>Explorary testing would be used to see if a user's moon is removed from the database upon successful deletion</t>
+  </si>
+  <si>
     <t>Error Guess testing would be used to check if passwords are hidden when an user inputs one when logging in to their account</t>
   </si>
   <si>
@@ -378,6 +396,9 @@
     <t>Equivalence Partitioning testing would be used to check if usernames have to be unique when creating an account</t>
   </si>
   <si>
+    <t>Exploratary testing would be used to check if an user's planets and moons are their own by looking at the database</t>
+  </si>
+  <si>
     <t>Acceptance testing would be used to see if creating a planet on the home page provides a good user experience (easy to use, intutitive, etc.)</t>
   </si>
   <si>
@@ -439,6 +460,9 @@
   </si>
   <si>
     <t>Sprint 2: Automation Testing</t>
+  </si>
+  <si>
+    <t>Sprint 3: Unit + Integration Testing</t>
   </si>
 </sst>
 </file>
@@ -448,7 +472,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yyyy"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -469,6 +493,10 @@
       <color theme="0"/>
       <name val="Arial"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="8">
@@ -551,15 +579,15 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="27">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
+      <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
+      <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="1" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
@@ -570,10 +598,10 @@
     <xf borderId="3" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="1" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="2" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="2" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="2" fillId="5" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -594,6 +622,18 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="4" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="2" fillId="4" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
@@ -616,6 +656,9 @@
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="6" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -901,7 +944,9 @@
       <c r="A3" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="4"/>
+      <c r="B3" s="5" t="s">
+        <v>9</v>
+      </c>
       <c r="C3" s="4" t="s">
         <v>11</v>
       </c>
@@ -922,305 +967,299 @@
       <c r="A4" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="4"/>
+      <c r="B4" s="6" t="s">
+        <v>14</v>
+      </c>
       <c r="C4" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>11</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>9</v>
+        <v>18</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>19</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="5"/>
+      <c r="E5" s="7" t="s">
+        <v>21</v>
+      </c>
       <c r="F5" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G5" s="5"/>
+        <v>22</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="6">
-      <c r="A6" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>22</v>
+      <c r="A6" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>26</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="B7" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="G7" s="7" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="C8" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="E8" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="F8" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="G8" s="9" t="s">
+      <c r="D8" s="6" t="s">
         <v>37</v>
       </c>
+      <c r="E8" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="G8" s="10" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="9">
-      <c r="A9" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="B9" s="9" t="s">
+      <c r="A9" s="6" t="s">
         <v>39</v>
       </c>
+      <c r="B9" s="11" t="s">
+        <v>40</v>
+      </c>
       <c r="C9" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="D9" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="E9" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="F9" s="7" t="s">
+      <c r="D9" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="G9" s="10" t="s">
-        <v>25</v>
+      <c r="E9" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="G9" s="11" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="B10" s="10" t="s">
-        <v>21</v>
+        <v>46</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>40</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>45</v>
+        <v>47</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>48</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="F10" s="7" t="s">
-        <v>47</v>
+        <v>49</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>50</v>
       </c>
       <c r="G10" s="11" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="E11" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="F11" s="7" t="s">
+      <c r="C11" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="G11" s="11" t="s">
+      <c r="D11" s="6" t="s">
         <v>54</v>
+      </c>
+      <c r="E11" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="G11" s="12" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="B12" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>56</v>
+        <v>58</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>60</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="E12" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="F12" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="G12" s="12" t="s">
-        <v>60</v>
+        <v>61</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="B13" s="12" t="s">
-        <v>62</v>
+        <v>63</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>64</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="F13" s="7" t="s">
-        <v>65</v>
+        <v>66</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="C14" s="6" t="s">
         <v>68</v>
       </c>
+      <c r="B14" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>70</v>
+      </c>
       <c r="D14" s="11" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="C15" s="7" t="s">
         <v>73</v>
       </c>
+      <c r="B15" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>74</v>
+      </c>
       <c r="D15" s="11" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="F15" s="10" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="B16" s="9" t="s">
         <v>76</v>
       </c>
+      <c r="B16" s="11" t="s">
+        <v>77</v>
+      </c>
       <c r="C16" s="9" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D16" s="11" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F16" s="11" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="12" t="s">
-        <v>80</v>
-      </c>
-      <c r="B17" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="C17" s="6" t="s">
         <v>81</v>
       </c>
+      <c r="B17" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>83</v>
+      </c>
       <c r="D17" s="12" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="F17" s="11" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="13"/>
-      <c r="B18" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="C18" s="7" t="s">
-        <v>56</v>
+      <c r="C18" s="6" t="s">
+        <v>60</v>
       </c>
       <c r="F18" s="11" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="13"/>
-      <c r="B19" s="12" t="s">
-        <v>86</v>
-      </c>
       <c r="C19" s="9" t="s">
         <v>87</v>
       </c>
@@ -1229,7 +1268,7 @@
       </c>
     </row>
     <row r="20">
-      <c r="C20" s="6" t="s">
+      <c r="C20" s="7" t="s">
         <v>89</v>
       </c>
       <c r="F20" s="11" t="s">
@@ -1237,7 +1276,7 @@
       </c>
     </row>
     <row r="21">
-      <c r="C21" s="7" t="s">
+      <c r="C21" s="6" t="s">
         <v>91</v>
       </c>
       <c r="F21" s="12" t="s">
@@ -1274,144 +1313,160 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="15" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
+      <c r="A2" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>95</v>
+      </c>
       <c r="C2" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
+        <v>96</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="E2" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="F2" s="16" t="s">
+        <v>99</v>
+      </c>
+      <c r="G2" s="16" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="3">
-      <c r="A3" s="4"/>
+      <c r="A3" s="17" t="s">
+        <v>95</v>
+      </c>
       <c r="B3" s="4" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="4" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="4" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="4" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="C7" s="4"/>
+        <v>126</v>
+      </c>
+      <c r="C7" s="17" t="s">
+        <v>127</v>
+      </c>
       <c r="D7" s="5" t="s">
-        <v>121</v>
+        <v>128</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>122</v>
+        <v>129</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="5" t="s">
-        <v>123</v>
+        <v>130</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>124</v>
+        <v>131</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>125</v>
+        <v>132</v>
       </c>
     </row>
   </sheetData>
@@ -1433,199 +1488,292 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="14" t="s">
-        <v>126</v>
-      </c>
-      <c r="B1" s="14" t="s">
-        <v>127</v>
-      </c>
-      <c r="C1" s="14" t="s">
-        <v>128</v>
-      </c>
-      <c r="E1" s="14" t="s">
-        <v>129</v>
+      <c r="A1" s="18" t="s">
+        <v>133</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>134</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>135</v>
+      </c>
+      <c r="E1" s="18" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="14" t="s">
-        <v>130</v>
-      </c>
-      <c r="B2" s="15">
+      <c r="A2" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="B2" s="19">
         <v>45580.0</v>
       </c>
-      <c r="C2" s="15">
+      <c r="C2" s="19">
         <v>45581.0</v>
       </c>
-      <c r="E2" s="16" t="s">
-        <v>131</v>
+      <c r="E2" s="20" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="14" t="s">
-        <v>132</v>
-      </c>
-      <c r="B3" s="15">
+      <c r="A3" s="18" t="s">
+        <v>139</v>
+      </c>
+      <c r="B3" s="19">
         <v>45582.0</v>
       </c>
-      <c r="C3" s="17">
+      <c r="C3" s="21">
         <v>45583.0</v>
       </c>
-      <c r="E3" s="18" t="s">
+      <c r="E3" s="22" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="18" t="s">
+        <v>141</v>
+      </c>
+      <c r="B4" s="23">
+        <v>45584.0</v>
+      </c>
+      <c r="C4" s="23">
+        <v>45589.0</v>
+      </c>
+      <c r="E4" s="24" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="18" t="s">
+        <v>143</v>
+      </c>
+      <c r="B5" s="23">
+        <v>45590.0</v>
+      </c>
+      <c r="C5" s="23">
+        <v>45591.0</v>
+      </c>
+      <c r="E5" s="25" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="18" t="s">
+        <v>145</v>
+      </c>
+      <c r="B6" s="23">
+        <v>45591.0</v>
+      </c>
+      <c r="C6" s="23">
+        <v>45593.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="18" t="s">
+        <v>146</v>
+      </c>
+      <c r="B7" s="19">
+        <v>45594.0</v>
+      </c>
+      <c r="C7" s="19">
+        <v>45597.0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="18" t="s">
+        <v>147</v>
+      </c>
+      <c r="B9" s="19">
+        <v>45580.0</v>
+      </c>
+      <c r="C9" s="19">
+        <v>45597.0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="18" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="18" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="14" t="s">
+      <c r="B12" s="18" t="s">
         <v>134</v>
       </c>
-      <c r="B4" s="19">
-        <v>45584.0</v>
-      </c>
-      <c r="C4" s="19">
-        <v>45589.0</v>
-      </c>
-      <c r="E4" s="20" t="s">
+      <c r="C12" s="18" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" s="14" t="s">
-        <v>136</v>
-      </c>
-      <c r="B5" s="19">
-        <v>45590.0</v>
-      </c>
-      <c r="C5" s="19">
-        <v>45591.0</v>
-      </c>
-      <c r="E5" s="21" t="s">
+    <row r="13">
+      <c r="A13" s="18" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="14" t="s">
-        <v>138</v>
-      </c>
-      <c r="B6" s="19">
-        <v>45591.0</v>
-      </c>
-      <c r="C6" s="19">
-        <v>45593.0</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="14" t="s">
+      <c r="B13" s="19">
+        <v>45600.0</v>
+      </c>
+      <c r="C13" s="19">
+        <v>45602.0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="18" t="s">
         <v>139</v>
       </c>
-      <c r="B7" s="15">
-        <v>45594.0</v>
-      </c>
-      <c r="C7" s="15">
-        <v>45597.0</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="14" t="s">
-        <v>140</v>
-      </c>
-      <c r="B9" s="15">
-        <v>45580.0</v>
-      </c>
-      <c r="C9" s="15">
-        <v>45597.0</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="14" t="s">
+      <c r="B14" s="19">
+        <v>45602.0</v>
+      </c>
+      <c r="C14" s="19">
+        <v>45602.0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="18" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="14" t="s">
-        <v>126</v>
-      </c>
-      <c r="B12" s="14" t="s">
-        <v>127</v>
-      </c>
-      <c r="C12" s="14" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="14" t="s">
-        <v>130</v>
-      </c>
-      <c r="B13" s="15">
+      <c r="B15" s="19">
+        <v>45602.0</v>
+      </c>
+      <c r="C15" s="19">
+        <v>45604.0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="18" t="s">
+        <v>143</v>
+      </c>
+      <c r="B16" s="21">
+        <v>45605.0</v>
+      </c>
+      <c r="C16" s="21">
+        <v>45608.0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="18" t="s">
+        <v>145</v>
+      </c>
+      <c r="B17" s="21">
+        <v>45609.0</v>
+      </c>
+      <c r="C17" s="19">
+        <v>45610.0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="18" t="s">
+        <v>146</v>
+      </c>
+      <c r="B18" s="19">
+        <v>45610.0</v>
+      </c>
+      <c r="C18" s="19">
+        <v>45611.0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="18" t="s">
+        <v>147</v>
+      </c>
+      <c r="B20" s="19">
         <v>45600.0</v>
       </c>
-      <c r="C13" s="15">
-        <v>45602.0</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="14" t="s">
-        <v>132</v>
-      </c>
-      <c r="B14" s="15">
-        <v>45602.0</v>
-      </c>
-      <c r="C14" s="15">
-        <v>45602.0</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="14" t="s">
+      <c r="C20" s="19">
+        <v>45611.0</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="18" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="18" t="s">
+        <v>133</v>
+      </c>
+      <c r="B23" s="18" t="s">
         <v>134</v>
       </c>
-      <c r="B15" s="15">
-        <v>45602.0</v>
-      </c>
-      <c r="C15" s="15">
-        <v>45604.0</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="14" t="s">
-        <v>136</v>
-      </c>
-      <c r="B16" s="17">
-        <v>45605.0</v>
-      </c>
-      <c r="C16" s="17">
-        <v>45608.0</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="14" t="s">
-        <v>138</v>
-      </c>
-      <c r="B17" s="17">
-        <v>45609.0</v>
-      </c>
-      <c r="C17" s="15">
-        <v>45610.0</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="14" t="s">
+      <c r="C23" s="18" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="B24" s="19">
+        <v>45615.0</v>
+      </c>
+      <c r="C24" s="19">
+        <v>45615.0</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="18" t="s">
         <v>139</v>
       </c>
-      <c r="B18" s="15">
-        <v>45610.0</v>
-      </c>
-      <c r="C18" s="15">
-        <v>45611.0</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="14" t="s">
-        <v>140</v>
-      </c>
-      <c r="B20" s="15">
-        <v>45600.0</v>
-      </c>
-      <c r="C20" s="15">
-        <v>45611.0</v>
+      <c r="B25" s="19">
+        <v>45615.0</v>
+      </c>
+      <c r="C25" s="19">
+        <v>45615.0</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="18" t="s">
+        <v>141</v>
+      </c>
+      <c r="B26" s="19">
+        <v>45615.0</v>
+      </c>
+      <c r="C26" s="26">
+        <v>45621.0</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="18" t="s">
+        <v>143</v>
+      </c>
+      <c r="B27" s="19">
+        <v>45621.0</v>
+      </c>
+      <c r="C27" s="19">
+        <v>45621.0</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="18" t="s">
+        <v>145</v>
+      </c>
+      <c r="B28" s="23">
+        <v>45621.0</v>
+      </c>
+      <c r="C28" s="19">
+        <v>45622.0</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="18" t="s">
+        <v>146</v>
+      </c>
+      <c r="B29" s="19">
+        <v>45622.0</v>
+      </c>
+      <c r="C29" s="19">
+        <v>45623.0</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="18" t="s">
+        <v>147</v>
+      </c>
+      <c r="B31" s="23">
+        <v>45614.0</v>
+      </c>
+      <c r="C31" s="19">
+        <v>45623.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>